<commit_message>
added kmeans clustering to visually view the clusters
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20406"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonly\OneDrive\Coding Stuff\Project Ideas\NPI specialty clustering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonly\Documents\GitHub\NPI-Specialty-Clustering-and-Prediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="4_{A02754E1-7231-4A5C-8018-E29868060A33}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{915FA9CF-68B9-47A6-8944-4CEC1697528E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F72DEF0-343C-4040-A3B4-168EFAFFB225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="14">
   <si>
     <t>rx_id</t>
   </si>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D84"/>
+  <dimension ref="A1:D86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -509,7 +509,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -523,7 +523,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
@@ -761,7 +761,7 @@
         <v>7</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -845,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -873,7 +873,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -881,13 +881,13 @@
         <v>34</v>
       </c>
       <c r="B35" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -895,7 +895,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>10</v>
@@ -915,7 +915,7 @@
         <v>10</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -929,7 +929,7 @@
         <v>10</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -943,7 +943,7 @@
         <v>10</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -951,13 +951,13 @@
         <v>39</v>
       </c>
       <c r="B40" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -965,13 +965,13 @@
         <v>40</v>
       </c>
       <c r="B41" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1013,7 +1013,7 @@
         <v>11</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1027,7 +1027,7 @@
         <v>11</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1077,13 +1077,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1091,13 +1091,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1153,7 +1153,7 @@
         <v>11</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1167,7 +1167,7 @@
         <v>11</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1175,13 +1175,13 @@
         <v>55</v>
       </c>
       <c r="B56" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1189,13 +1189,13 @@
         <v>56</v>
       </c>
       <c r="B57" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1209,7 +1209,7 @@
         <v>12</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -1223,7 +1223,7 @@
         <v>12</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -1273,7 +1273,7 @@
         <v>62</v>
       </c>
       <c r="B63" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>12</v>
@@ -1287,7 +1287,7 @@
         <v>63</v>
       </c>
       <c r="B64" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>12</v>
@@ -1321,7 +1321,7 @@
         <v>12</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1343,13 +1343,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1357,13 +1357,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.3">
@@ -1391,7 +1391,7 @@
         <v>13</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1405,7 +1405,7 @@
         <v>13</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,13 +1413,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1427,13 +1427,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1483,13 +1483,13 @@
         <v>77</v>
       </c>
       <c r="B78" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1497,16 +1497,19 @@
         <v>78</v>
       </c>
       <c r="B79" s="1">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
       <c r="B80" s="1">
         <v>13</v>
       </c>
@@ -1517,7 +1520,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
       <c r="B81" s="1">
         <v>13</v>
       </c>
@@ -1528,7 +1534,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
       <c r="B82" s="1">
         <v>13</v>
       </c>
@@ -1539,7 +1548,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
       <c r="B83" s="1">
         <v>13</v>
       </c>
@@ -1547,10 +1559,13 @@
         <v>5</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
       <c r="B84" s="1">
         <v>13</v>
       </c>
@@ -1558,6 +1573,34 @@
         <v>5</v>
       </c>
       <c r="D84" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="1">
+        <v>13</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="1">
+        <v>13</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D86" s="1" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>